<commit_message>
docs: End of Forecast Month Jun 19th
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21480"/>
+    <workbookView windowHeight="21480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="149">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -334,7 +334,7 @@
     <t>Mother Air Ticket</t>
   </si>
   <si>
-    <t>Mother Amazon Books</t>
+    <t>Mother Borrowed Credit Card</t>
   </si>
   <si>
     <t>Total Debts</t>
@@ -394,14 +394,16 @@
   <si>
     <t>1. Mother borrowed $570 For Buying Cigarette Buds.
 2. Mother give $100 For Lunch (Without Paying Back).
-3. Mother borrowed $150.9 For online Amazon Book Store.</t>
+3. Provide Credit Card For purchasing books From Amazon. (Don't need to Include because it is included in the Debts) ~ $150.9</t>
   </si>
   <si>
     <t>1. N/A ~ $2435
 2. Additional Half Month Allowance ~ $1048</t>
   </si>
   <si>
-    <t>1. Give $50 For seeing Doctor at Wu York Yu</t>
+    <t>1. Provide Credit Card For puchasing Bayer Aspirin From SpringSunday  (Don't need to Include because it is included in the Debts). ~ $276.04
+2. Give $50 For seeing Doctor at Wu York Yu
+3. Provide Credit Card For purchasing Body Lotion and Hair Dyeing Products From Amazon. (Don't need to Include because it is included in the Debts). ~ $537.79</t>
   </si>
   <si>
     <t>1. Sportify
@@ -420,11 +422,14 @@
 2. Stop Services ~ 19.99</t>
   </si>
   <si>
-    <t>Octopus</t>
+    <t>1. Octopus
+2. Octopus
+3. Google PlayStore</t>
   </si>
   <si>
     <t>1. 20th May 2025 -  Top Up For Octopus $50 (Don't need to Include)
-2. 23rd May 2025 -  Top Up For Octopus $100 (Don't need to Include)</t>
+2. 23rd May 2025 -  Top Up For Octopus $100 (Don't need to Include)
+3. 19th June 2025 -  Top Up For PlayStore $150 (Don't need to Include)</t>
   </si>
   <si>
     <t>yuu</t>
@@ -441,12 +446,6 @@
   </si>
   <si>
     <t>Cancel Oxford Dictionary Subscription</t>
-  </si>
-  <si>
-    <t>Google PlayStore</t>
-  </si>
-  <si>
-    <t>1. 20th June 2025 -  Top Up For PlayStore $150 (Don't need to Include)</t>
   </si>
   <si>
     <t>- See the Doctor ~ $110
@@ -468,13 +467,12 @@
 ~ Coke From Machine ~ $6.5</t>
   </si>
   <si>
-    <t>~ Amazon Book Store ~ $150.9</t>
-  </si>
-  <si>
     <t xml:space="preserve">~ Payback $570 to Mom </t>
   </si>
   <si>
-    <t>~ Payback $150.9 to Mom</t>
+    <t>1.  Payback $276.04 to Mom For paying Bayer Aspirin Brought From SpringSunday.com 
+2. Payback $150.9 to Mom For paying Amazon Books. 
+3. Payback the remaining $10.46 after spending from Amazon Gift card (due to refund). For purchasing Body Lotion and Hair Dyeing Products From Amazon.</t>
   </si>
   <si>
     <t>~ See the Doctor (Injection) ~ $19
@@ -491,7 +489,8 @@
     <t>~ Apple Music 2 month
 ~ Top Up For Mobile And Comunication ~ $0.6
 ~ 20th May 2025 - Top Up For Octopus $50 (Don't need to Include)
-~ 23rd May 2025 - Top Up For Octopus $100 (Don't need to Include)</t>
+~ 23rd May 2025 - Top Up For Octopus $100 (Don't need to Include)
+~  Top Up For PlayStore $150 (Don't need to Include)</t>
   </si>
   <si>
     <t>~ Food And Transport
@@ -509,7 +508,9 @@
   - Best Mart ~ soft drinks $18
   - Best Mart ~ Starbucks Coffee Beans ~ $49.9
   - Wellcome ~ Sugar ~ $6.5
-  - U Mart ~ Nisan Noddle and Curd Beans ~ $20.8</t>
+  - U Mart ~ Nisan Noddle and Curd Beans ~ $20.8
+  - Best Mart 360 ~ Coffee Beans $49
+  - CY Market Bakery ~ $28</t>
   </si>
   <si>
     <t>~ Nivea body lotion 380ml ~ $32
@@ -526,8 +527,9 @@
 ~ Round Trip to East Kowloon Hospital ~ $4
 ~ Watsons ~ Asprin Like medicine ~ $49
 ~ Wellcome ~ Plastic bag ~ $1
-~ Spring Sunday Aspirin tablets ~ $276.04
-~ Chuk Yuen North Post Office ~ stamp $2.2</t>
+~ Chuk Yuen North Post Office ~ stamp $2.2
+~ Medimart 3M TEGADERM 10 pieces ~ $60
+~ CY Plaza 2nd Pharmacy ~ Cotten buds ~ $10</t>
   </si>
   <si>
     <t>Balance Brought Forward From July 2024</t>
@@ -536,15 +538,14 @@
     <t>~ Payback $700 to Mom</t>
   </si>
   <si>
+    <t>~ Payback $527.51 to Mom For Purchasing Amazon Body Lotion and hair dying solutions.</t>
+  </si>
+  <si>
     <t>- See the Doctor ~ $110
-- Buy Cigarette Buds ~ $800
-~ Transport for Cigarette Buds ~ $50</t>
+- Buy Cigarette Buds ~ $650</t>
   </si>
   <si>
     <t>~ Food And Transport ~ $400</t>
-  </si>
-  <si>
-    <t>~ 20th June 2025 -  Top Up For PlayStore $150 (Don't need to Include)</t>
   </si>
   <si>
     <t>~ Payback $1050 to Mom</t>
@@ -566,10 +567,6 @@
   </si>
   <si>
     <t>~ Payback $1000 to Mom</t>
-  </si>
-  <si>
-    <t>- See the Doctor ~ $110
-- Buy Cigarette Buds ~ $650</t>
   </si>
   <si>
     <t>~ Payback $770 to Mom</t>
@@ -2397,6 +2394,9 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="25" xfId="52" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="22" xfId="52" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="26" xfId="52" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2531,9 +2531,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3139,7 +3136,7 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
@@ -4936,7 +4933,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -4952,7 +4949,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17738.78</v>
+        <v>17781.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -4968,7 +4965,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18202.56</v>
+        <v>18087.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -4984,7 +4981,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -6595,7 +6592,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -6603,7 +6600,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -6679,7 +6676,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -6695,7 +6692,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -6789,7 +6786,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>15509.78</v>
+        <v>15552.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -6958,7 +6955,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -6973,7 +6970,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -7061,7 +7058,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>16265.78</v>
+        <v>16308.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7153,7 +7150,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>16265.78</v>
+        <v>16308.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -7322,7 +7319,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -7337,7 +7334,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -7425,7 +7422,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17132.78</v>
+        <v>17175.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -7517,7 +7514,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>17132.78</v>
+        <v>17175.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -7686,7 +7683,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -7701,7 +7698,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -7789,7 +7786,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17738.78</v>
+        <v>17781.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -8305,7 +8302,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -8321,7 +8318,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>20388.78</v>
+        <v>20431.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -8337,7 +8334,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>20852.56</v>
+        <v>20737.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -8353,7 +8350,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -9964,7 +9961,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -9972,7 +9969,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -10048,7 +10045,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -10064,7 +10061,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -10158,7 +10155,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>17738.78</v>
+        <v>17781.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -10327,7 +10324,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -10342,7 +10339,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -10430,7 +10427,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>18765.78</v>
+        <v>18808.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -10522,7 +10519,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>18765.78</v>
+        <v>18808.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -10691,7 +10688,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -10706,7 +10703,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -10794,7 +10791,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19361.78</v>
+        <v>19404.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -10886,7 +10883,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>19361.78</v>
+        <v>19404.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11055,7 +11052,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -11070,7 +11067,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -11158,7 +11155,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>20388.78</v>
+        <v>20431.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -11670,7 +11667,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -11686,7 +11683,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>24121.78</v>
+        <v>24164.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -11702,7 +11699,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>24585.56</v>
+        <v>24470.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -11718,7 +11715,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -11970,7 +11967,7 @@
       </c>
       <c r="C23" s="98"/>
       <c r="D23" s="99" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E23" s="100"/>
       <c r="F23" s="7">
@@ -13333,7 +13330,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -13341,7 +13338,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -13417,7 +13414,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -13433,7 +13430,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -13527,7 +13524,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>20388.78</v>
+        <v>20431.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -13696,7 +13693,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -13711,7 +13708,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -13799,7 +13796,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>21415.78</v>
+        <v>21458.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -13891,7 +13888,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>21415.78</v>
+        <v>21458.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14060,7 +14057,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -14075,7 +14072,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -14163,7 +14160,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>23094.78</v>
+        <v>23137.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -14255,7 +14252,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>23094.78</v>
+        <v>23137.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -14424,7 +14421,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -14439,7 +14436,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -14527,7 +14524,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>24121.78</v>
+        <v>24164.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15045,7 +15042,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15061,7 +15058,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>26350.78</v>
+        <v>26393.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15077,7 +15074,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>26814.56</v>
+        <v>26699.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -15093,7 +15090,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -16704,7 +16701,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -16712,7 +16709,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -16788,7 +16785,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -16804,7 +16801,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -16898,7 +16895,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>24121.78</v>
+        <v>24164.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -17067,7 +17064,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -17082,7 +17079,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -17170,7 +17167,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>24877.78</v>
+        <v>24920.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -17262,7 +17259,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>24877.78</v>
+        <v>24920.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -17431,7 +17428,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -17446,7 +17443,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -17534,7 +17531,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>25744.78</v>
+        <v>25787.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -17626,7 +17623,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>25744.78</v>
+        <v>25787.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -17795,7 +17792,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -17810,7 +17807,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -17898,7 +17895,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>26350.78</v>
+        <v>26393.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -18415,7 +18412,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -18431,7 +18428,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>29000.78</v>
+        <v>29043.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -18447,7 +18444,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>29464.56</v>
+        <v>29349.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -18463,7 +18460,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -20074,7 +20071,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -20082,7 +20079,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -20158,7 +20155,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -20174,7 +20171,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -20268,7 +20265,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>26350.78</v>
+        <v>26393.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -20437,7 +20434,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -20452,7 +20449,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -20540,7 +20537,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>27377.78</v>
+        <v>27420.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -20632,7 +20629,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>27377.78</v>
+        <v>27420.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -20801,7 +20798,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -20816,7 +20813,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -20904,7 +20901,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>27973.78</v>
+        <v>28016.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -20996,7 +20993,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>27973.78</v>
+        <v>28016.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -21165,7 +21162,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -21180,7 +21177,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -21268,7 +21265,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>29000.78</v>
+        <v>29043.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -21778,7 +21775,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -21794,7 +21791,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>31319.78</v>
+        <v>31362.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -21810,7 +21807,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>31783.56</v>
+        <v>31668.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -21826,7 +21823,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -23437,7 +23434,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -23445,7 +23442,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -23521,7 +23518,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -23537,7 +23534,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -23631,7 +23628,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>29000.78</v>
+        <v>29043.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -23800,7 +23797,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -23815,7 +23812,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -23903,7 +23900,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>29806.78</v>
+        <v>29849.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -23995,7 +23992,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>29806.78</v>
+        <v>29849.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -24164,7 +24161,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -24179,7 +24176,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -24267,7 +24264,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>30673.78</v>
+        <v>30716.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -24359,7 +24356,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>30673.78</v>
+        <v>30716.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -24528,7 +24525,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -24543,7 +24540,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -24631,7 +24628,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>31319.78</v>
+        <v>31362.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -25147,7 +25144,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -25163,7 +25160,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35052.78</v>
+        <v>35095.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -25179,7 +25176,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35516.56</v>
+        <v>35401.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -25195,7 +25192,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -25447,7 +25444,7 @@
       </c>
       <c r="C23" s="98"/>
       <c r="D23" s="99" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E23" s="100"/>
       <c r="F23" s="7">
@@ -26810,7 +26807,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -26818,7 +26815,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -26894,7 +26891,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -26910,7 +26907,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -27004,7 +27001,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>31319.78</v>
+        <v>31362.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -27173,7 +27170,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -27188,7 +27185,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -27276,7 +27273,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>32346.78</v>
+        <v>32389.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -27368,7 +27365,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>32346.78</v>
+        <v>32389.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -27537,7 +27534,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -27552,7 +27549,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -27640,7 +27637,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>34025.78</v>
+        <v>34068.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -27732,7 +27729,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>34025.78</v>
+        <v>34068.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -27901,7 +27898,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -27916,7 +27913,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -28004,7 +28001,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35052.78</v>
+        <v>35095.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -28501,7 +28498,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -28517,7 +28514,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>37481.78</v>
+        <v>37524.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -28533,7 +28530,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>37945.56</v>
+        <v>37830.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28549,7 +28546,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -30123,7 +30120,7 @@
         <v>Bankruptcy Department / Government</v>
       </c>
       <c r="B102" s="38" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
@@ -30159,7 +30156,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -30167,7 +30164,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -30243,7 +30240,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -30259,7 +30256,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -30353,7 +30350,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>35052.78</v>
+        <v>35095.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -30522,7 +30519,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -30537,7 +30534,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -30625,7 +30622,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35858.78</v>
+        <v>35901.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -30717,7 +30714,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>35858.78</v>
+        <v>35901.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -30886,7 +30883,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -30901,7 +30898,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -30989,7 +30986,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>36725.78</v>
+        <v>36768.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -31081,7 +31078,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>36725.78</v>
+        <v>36768.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -31250,7 +31247,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -31265,7 +31262,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -31353,7 +31350,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>37481.78</v>
+        <v>37524.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -31857,7 +31854,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -31873,7 +31870,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>40131.78</v>
+        <v>40174.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -31889,7 +31886,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>40595.56</v>
+        <v>40480.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31905,7 +31902,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -33516,7 +33513,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -33524,7 +33521,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -33600,7 +33597,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -33616,7 +33613,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -33710,7 +33707,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>37481.78</v>
+        <v>37524.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -33879,7 +33876,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -33894,7 +33891,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -33982,7 +33979,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>38508.78</v>
+        <v>38551.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -34074,7 +34071,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>38508.78</v>
+        <v>38551.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -34243,7 +34240,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -34258,7 +34255,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -34346,7 +34343,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>39104.78</v>
+        <v>39147.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -34438,7 +34435,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>39104.78</v>
+        <v>39147.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -34607,7 +34604,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -34622,7 +34619,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -34710,7 +34707,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>40131.78</v>
+        <v>40174.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -35712,37 +35709,37 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
   <cols>
-    <col min="1" max="1" width="18.875" style="151" customWidth="1"/>
-    <col min="2" max="2" width="25.625" style="151" customWidth="1"/>
-    <col min="3" max="4" width="20.625" style="151" customWidth="1"/>
-    <col min="5" max="5" width="25.625" style="151" customWidth="1"/>
-    <col min="6" max="6" width="20.625" style="151" customWidth="1"/>
-    <col min="7" max="7" width="9" style="151"/>
-    <col min="8" max="8" width="23" style="151" customWidth="1"/>
+    <col min="1" max="1" width="18.875" style="152" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="152" customWidth="1"/>
+    <col min="3" max="4" width="20.625" style="152" customWidth="1"/>
+    <col min="5" max="5" width="25.625" style="152" customWidth="1"/>
+    <col min="6" max="6" width="20.625" style="152" customWidth="1"/>
+    <col min="7" max="7" width="9" style="152"/>
+    <col min="8" max="8" width="23" style="152" customWidth="1"/>
     <col min="9" max="9" width="40.75" style="48" customWidth="1"/>
-    <col min="10" max="10" width="28.625" style="151" customWidth="1"/>
-    <col min="11" max="12" width="9" style="151"/>
-    <col min="13" max="13" width="36.625" style="151" customWidth="1"/>
-    <col min="14" max="14" width="21.125" style="151" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="151"/>
+    <col min="10" max="10" width="28.625" style="152" customWidth="1"/>
+    <col min="11" max="12" width="9" style="152"/>
+    <col min="13" max="13" width="36.625" style="152" customWidth="1"/>
+    <col min="14" max="14" width="21.125" style="152" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="152"/>
   </cols>
   <sheetData>
     <row r="1" ht="36.75" customHeight="1" spans="1:14">
-      <c r="A1" s="152" t="str">
+      <c r="A1" s="153" t="str">
         <f>"Forecasts For the Year "&amp;TEXT(Main!B3,"mmmm yyyy")&amp;" to "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,3)-1,"mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*3+2),"mmmm yyyy"))</f>
         <v>Forecasts For the Year January 2025 to April 2025</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
       <c r="I1" s="192" t="s">
         <v>25</v>
       </c>
@@ -35753,16 +35750,16 @@
       <c r="N1" s="192"/>
     </row>
     <row r="2" ht="36" customHeight="1" spans="1:14">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="154" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="154"/>
-      <c r="C2" s="154"/>
-      <c r="D2" s="155" t="s">
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="156" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
       <c r="I2" s="193" t="s">
         <v>29</v>
       </c>
@@ -35777,23 +35774,23 @@
       </c>
     </row>
     <row r="3" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="157" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="157" t="s">
+      <c r="B3" s="158" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="158">
-        <v>368</v>
-      </c>
-      <c r="D3" s="159" t="s">
+      <c r="C3" s="159">
+        <v>118.5</v>
+      </c>
+      <c r="D3" s="160" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="187">
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="I3" s="195" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*1,"dd mmmm yyyy"))</f>
@@ -35809,18 +35806,18 @@
       </c>
       <c r="N3" s="196">
         <f>-C122</f>
-        <v>-333923.41</v>
+        <v>-334737.42</v>
       </c>
     </row>
     <row r="4" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A4" s="156"/>
-      <c r="B4" s="157" t="s">
+      <c r="A4" s="157"/>
+      <c r="B4" s="158" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="158">
-        <v>0</v>
-      </c>
-      <c r="D4" s="160"/>
+      <c r="C4" s="159">
+        <v>0</v>
+      </c>
+      <c r="D4" s="161"/>
       <c r="E4" s="5" t="s">
         <v>35</v>
       </c>
@@ -35841,18 +35838,18 @@
       </c>
       <c r="N4" s="196">
         <f ca="1">'April 2025 - June 2025'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="5" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A5" s="156"/>
-      <c r="B5" s="157" t="s">
+      <c r="A5" s="157"/>
+      <c r="B5" s="158" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="158">
-        <v>0</v>
-      </c>
-      <c r="D5" s="160"/>
+      <c r="C5" s="159">
+        <v>0</v>
+      </c>
+      <c r="D5" s="161"/>
       <c r="E5" s="5" t="s">
         <v>36</v>
       </c>
@@ -35873,18 +35870,18 @@
       </c>
       <c r="N5" s="196">
         <f ca="1">'July 2025 - September 2025'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="6" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A6" s="156"/>
-      <c r="B6" s="157" t="s">
+      <c r="A6" s="157"/>
+      <c r="B6" s="158" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="158">
-        <v>0</v>
-      </c>
-      <c r="D6" s="160"/>
+      <c r="C6" s="159">
+        <v>0</v>
+      </c>
+      <c r="D6" s="161"/>
       <c r="E6" s="5" t="s">
         <v>37</v>
       </c>
@@ -35905,23 +35902,23 @@
       </c>
       <c r="N6" s="196">
         <f ca="1">'October 2025 - December 2025'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="7" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A7" s="156"/>
-      <c r="B7" s="157" t="s">
+      <c r="A7" s="157"/>
+      <c r="B7" s="158" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="158">
-        <v>57.96</v>
-      </c>
-      <c r="D7" s="160"/>
+      <c r="C7" s="159">
+        <v>0</v>
+      </c>
+      <c r="D7" s="161"/>
       <c r="E7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F7" s="187">
-        <v>357.96</v>
+        <v>32.96</v>
       </c>
       <c r="I7" s="198" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,4),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*4)+4,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,5)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*5+4),"dd mmmm yyyy"))</f>
@@ -35929,7 +35926,7 @@
       </c>
       <c r="J7" s="196">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="M7" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,12),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*12+12),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,15)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+14),"dd mmmm yyyy"))</f>
@@ -35937,18 +35934,18 @@
       </c>
       <c r="N7" s="196">
         <f ca="1">'January 2026 - March 2026'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="8" ht="45" customHeight="1" spans="1:14">
-      <c r="A8" s="156"/>
-      <c r="B8" s="157" t="s">
+      <c r="A8" s="157"/>
+      <c r="B8" s="158" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="158">
-        <v>0</v>
-      </c>
-      <c r="D8" s="160"/>
+      <c r="C8" s="159">
+        <v>0</v>
+      </c>
+      <c r="D8" s="161"/>
       <c r="E8" s="5" t="s">
         <v>39</v>
       </c>
@@ -35962,7 +35959,7 @@
       </c>
       <c r="J8" s="196">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>1188.78</v>
+        <v>1231.32</v>
       </c>
       <c r="M8" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,15),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+15),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,18)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+17),"dd mmmm yyyy"))</f>
@@ -35970,18 +35967,18 @@
       </c>
       <c r="N8" s="196">
         <f ca="1">'April 2026 - June 2026'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="9" ht="39.75" customHeight="1" spans="1:14">
-      <c r="A9" s="156"/>
-      <c r="B9" s="157" t="s">
+      <c r="A9" s="157"/>
+      <c r="B9" s="158" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="158">
-        <v>0</v>
-      </c>
-      <c r="D9" s="160"/>
+      <c r="C9" s="159">
+        <v>0</v>
+      </c>
+      <c r="D9" s="161"/>
       <c r="E9" s="5" t="s">
         <v>40</v>
       </c>
@@ -35994,7 +35991,7 @@
       </c>
       <c r="J9" s="196">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>2215.78</v>
+        <v>2258.32</v>
       </c>
       <c r="M9" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,18),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+18),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,21)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+20),"dd mmmm yyyy"))</f>
@@ -36002,18 +35999,18 @@
       </c>
       <c r="N9" s="205">
         <f ca="1">'July 2026 - September 2026'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="10" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A10" s="156"/>
-      <c r="B10" s="157" t="s">
+      <c r="A10" s="157"/>
+      <c r="B10" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="158">
-        <v>0</v>
-      </c>
-      <c r="D10" s="160"/>
+      <c r="C10" s="159">
+        <v>0</v>
+      </c>
+      <c r="D10" s="161"/>
       <c r="E10" s="5" t="s">
         <v>41</v>
       </c>
@@ -36026,7 +36023,7 @@
       </c>
       <c r="J10" s="196">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>3101.78</v>
+        <v>3144.32</v>
       </c>
       <c r="M10" s="206" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,21),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+21),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,24)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+23),"dd mmmm yyyy"))</f>
@@ -36034,18 +36031,18 @@
       </c>
       <c r="N10" s="196">
         <f ca="1">'October 2026 - December 2026'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="11" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A11" s="156"/>
-      <c r="B11" s="157" t="s">
+      <c r="A11" s="157"/>
+      <c r="B11" s="158" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="158">
-        <v>0</v>
-      </c>
-      <c r="D11" s="160"/>
+      <c r="C11" s="159">
+        <v>0</v>
+      </c>
+      <c r="D11" s="161"/>
       <c r="E11" s="5" t="s">
         <v>42</v>
       </c>
@@ -36059,7 +36056,7 @@
       </c>
       <c r="J11" s="196">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>4128.78</v>
+        <v>4171.32</v>
       </c>
       <c r="M11" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,24),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+24),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,27)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+26),"dd mmmm yyyy"))</f>
@@ -36067,18 +36064,18 @@
       </c>
       <c r="N11" s="200">
         <f ca="1">'January 2027 - March 2027'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="12" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A12" s="156"/>
-      <c r="B12" s="157" t="s">
+      <c r="A12" s="157"/>
+      <c r="B12" s="158" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="158">
-        <v>30.02</v>
-      </c>
-      <c r="D12" s="160"/>
+      <c r="C12" s="159">
+        <v>180.02</v>
+      </c>
+      <c r="D12" s="161"/>
       <c r="E12" s="189" t="s">
         <v>43</v>
       </c>
@@ -36091,7 +36088,7 @@
       </c>
       <c r="J12" s="196">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>5064.78</v>
+        <v>5107.32</v>
       </c>
       <c r="M12" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,27),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+27),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,30)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+29),"dd mmmm yyyy"))</f>
@@ -36099,23 +36096,23 @@
       </c>
       <c r="N12" s="200">
         <f ca="1">'April 2027 - June 2027'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="13" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A13" s="156"/>
-      <c r="B13" s="157" t="s">
+      <c r="A13" s="157"/>
+      <c r="B13" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="158">
+      <c r="C13" s="159">
         <v>4</v>
       </c>
-      <c r="D13" s="160"/>
+      <c r="D13" s="161"/>
       <c r="E13" s="189" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="187">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I13" s="199" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,10),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*10)+10,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,11)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*11+10),"dd mmmm yyyy"))</f>
@@ -36123,7 +36120,7 @@
       </c>
       <c r="J13" s="196">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>6041.78</v>
+        <v>6084.32</v>
       </c>
       <c r="M13" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,30),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+30),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,33)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+32),"dd mmmm yyyy"))</f>
@@ -36131,18 +36128,18 @@
       </c>
       <c r="N13" s="200">
         <f ca="1">'July 2027 - September 2027'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="14" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A14" s="156"/>
-      <c r="B14" s="157" t="s">
+      <c r="A14" s="157"/>
+      <c r="B14" s="158" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="158">
+      <c r="C14" s="159">
         <v>3.8</v>
       </c>
-      <c r="D14" s="160"/>
+      <c r="D14" s="161"/>
       <c r="E14" s="189" t="s">
         <v>45</v>
       </c>
@@ -36155,7 +36152,7 @@
       </c>
       <c r="J14" s="200">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>6847.78</v>
+        <v>6890.32</v>
       </c>
       <c r="M14" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -36163,18 +36160,18 @@
       </c>
       <c r="N14" s="200">
         <f ca="1">'October 2027 - December 2027'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="15" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A15" s="156"/>
-      <c r="B15" s="161" t="s">
+      <c r="A15" s="157"/>
+      <c r="B15" s="162" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="158">
-        <v>0</v>
-      </c>
-      <c r="D15" s="160"/>
+      <c r="C15" s="159">
+        <v>0</v>
+      </c>
+      <c r="D15" s="161"/>
       <c r="E15" s="189" t="s">
         <v>46</v>
       </c>
@@ -36187,7 +36184,7 @@
       </c>
       <c r="J15" s="200">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>7874.78</v>
+        <v>7917.32</v>
       </c>
       <c r="M15" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -36195,25 +36192,25 @@
       </c>
       <c r="N15" s="200">
         <f ca="1">'January 2028 - March 2028'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="16" ht="35.25" customHeight="1" spans="1:14">
-      <c r="A16" s="162"/>
-      <c r="B16" s="163" t="s">
+      <c r="A16" s="163"/>
+      <c r="B16" s="164" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="164">
+      <c r="C16" s="165">
         <f>SUM(C3:C15)</f>
-        <v>463.78</v>
-      </c>
-      <c r="D16" s="165"/>
-      <c r="E16" s="163" t="s">
+        <v>306.32</v>
+      </c>
+      <c r="D16" s="166"/>
+      <c r="E16" s="164" t="s">
         <v>47</v>
       </c>
       <c r="F16" s="190">
         <f>SUM(F3:F15)</f>
-        <v>394.78</v>
+        <v>326.78</v>
       </c>
       <c r="I16" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -36221,7 +36218,7 @@
       </c>
       <c r="J16" s="200">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>8470.78</v>
+        <v>8513.32</v>
       </c>
       <c r="M16" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -36229,7 +36226,7 @@
       </c>
       <c r="N16" s="200">
         <f ca="1">'April 2028 - June 2028'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="17" ht="35.25" customHeight="1" spans="9:14">
@@ -36239,7 +36236,7 @@
       </c>
       <c r="J17" s="200">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>9497.78</v>
+        <v>9540.32</v>
       </c>
       <c r="M17" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -36247,7 +36244,7 @@
       </c>
       <c r="N17" s="200">
         <f ca="1">'July 2028 - September 2028'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="18" ht="35.25" customHeight="1" spans="9:14">
@@ -36257,7 +36254,7 @@
       </c>
       <c r="J18" s="200">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>10253.78</v>
+        <v>10296.32</v>
       </c>
       <c r="M18" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -36265,7 +36262,7 @@
       </c>
       <c r="N18" s="196">
         <f ca="1">'October 2028 - December 2028'!C5</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
     </row>
     <row r="19" ht="33" customHeight="1" spans="9:10">
@@ -36275,7 +36272,7 @@
       </c>
       <c r="J19" s="200">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>12203.78</v>
+        <v>12246.32</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -36285,7 +36282,7 @@
       </c>
       <c r="J20" s="200">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>12859.78</v>
+        <v>12902.32</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -36295,7 +36292,7 @@
       </c>
       <c r="J21" s="200">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>13886.78</v>
+        <v>13929.32</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -36315,7 +36312,7 @@
       </c>
       <c r="J22" s="200">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>14482.78</v>
+        <v>14525.32</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -36340,15 +36337,15 @@
       </c>
       <c r="J23" s="200">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>15509.78</v>
+        <v>15552.32</v>
       </c>
     </row>
     <row r="24" ht="33" customHeight="1" spans="1:10">
       <c r="A24" s="19"/>
-      <c r="B24" s="166"/>
-      <c r="C24" s="167"/>
-      <c r="D24" s="167"/>
-      <c r="E24" s="167"/>
+      <c r="B24" s="167"/>
+      <c r="C24" s="168"/>
+      <c r="D24" s="168"/>
+      <c r="E24" s="168"/>
       <c r="F24" s="43">
         <v>0</v>
       </c>
@@ -36359,7 +36356,7 @@
       </c>
       <c r="J24" s="200">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>16265.78</v>
+        <v>16308.32</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -36378,7 +36375,7 @@
       </c>
       <c r="J25" s="200">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>17132.78</v>
+        <v>17175.32</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -36397,7 +36394,7 @@
       </c>
       <c r="J26" s="200">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>17738.78</v>
+        <v>17781.32</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -36416,7 +36413,7 @@
       </c>
       <c r="J27" s="200">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>18765.78</v>
+        <v>18808.32</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -36435,7 +36432,7 @@
       </c>
       <c r="J28" s="200">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>19361.78</v>
+        <v>19404.32</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -36454,13 +36451,13 @@
       </c>
       <c r="J29" s="196">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>20388.78</v>
+        <v>20431.32</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
-      <c r="A30" s="168"/>
-      <c r="B30" s="169"/>
-      <c r="C30" s="170"/>
+      <c r="A30" s="169"/>
+      <c r="B30" s="170"/>
+      <c r="C30" s="171"/>
       <c r="D30" s="28" t="s">
         <v>51</v>
       </c>
@@ -36476,7 +36473,7 @@
       </c>
       <c r="J30" s="202">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>21415.78</v>
+        <v>21458.32</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -36486,7 +36483,7 @@
       </c>
       <c r="J31" s="200">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>23094.78</v>
+        <v>23137.32</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -36496,7 +36493,7 @@
       </c>
       <c r="J32" s="200">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>24121.78</v>
+        <v>24164.32</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -36506,7 +36503,7 @@
       </c>
       <c r="J33" s="200">
         <f ca="1">'July 2027 - September 2027'!E136</f>
-        <v>24877.78</v>
+        <v>24920.32</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -36526,7 +36523,7 @@
       </c>
       <c r="J34" s="200">
         <f ca="1">'July 2027 - September 2027'!E163</f>
-        <v>25744.78</v>
+        <v>25787.32</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -36551,7 +36548,7 @@
       </c>
       <c r="J35" s="200">
         <f ca="1">'July 2027 - September 2027'!E190</f>
-        <v>26350.78</v>
+        <v>26393.32</v>
       </c>
     </row>
     <row r="36" ht="22" customHeight="1" spans="1:10">
@@ -36574,7 +36571,7 @@
       </c>
       <c r="J36" s="200">
         <f ca="1">'October 2027 - December 2027'!E136</f>
-        <v>27377.78</v>
+        <v>27420.32</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -36593,12 +36590,12 @@
       </c>
       <c r="J37" s="200">
         <f ca="1">'October 2027 - December 2027'!E163</f>
-        <v>27973.78</v>
+        <v>28016.32</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
       <c r="A38" s="19"/>
-      <c r="B38" s="171"/>
+      <c r="B38" s="172"/>
       <c r="C38" s="23"/>
       <c r="D38" s="22"/>
       <c r="E38" s="23"/>
@@ -36612,7 +36609,7 @@
       </c>
       <c r="J38" s="200">
         <f ca="1">'October 2027 - December 2027'!E190</f>
-        <v>29000.78</v>
+        <v>29043.32</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -36631,7 +36628,7 @@
       </c>
       <c r="J39" s="200">
         <f ca="1">'January 2028 - March 2028'!E136</f>
-        <v>29806.78</v>
+        <v>29849.32</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -36650,7 +36647,7 @@
       </c>
       <c r="J40" s="200">
         <f ca="1">'January 2028 - March 2028'!E163</f>
-        <v>30673.78</v>
+        <v>30716.32</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -36669,13 +36666,13 @@
       </c>
       <c r="J41" s="200">
         <f ca="1">'January 2028 - March 2028'!E190</f>
-        <v>31319.78</v>
+        <v>31362.32</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
-      <c r="A42" s="168"/>
-      <c r="B42" s="169"/>
-      <c r="C42" s="170"/>
+      <c r="A42" s="169"/>
+      <c r="B42" s="170"/>
+      <c r="C42" s="171"/>
       <c r="D42" s="28" t="s">
         <v>51</v>
       </c>
@@ -36691,7 +36688,7 @@
       </c>
       <c r="J42" s="200">
         <f ca="1">'April 2028 - June 2028'!E136</f>
-        <v>32346.78</v>
+        <v>32389.32</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -36701,7 +36698,7 @@
       </c>
       <c r="J43" s="200">
         <f ca="1">'April 2028 - June 2028'!E163</f>
-        <v>34025.78</v>
+        <v>34068.32</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -36711,7 +36708,7 @@
       </c>
       <c r="J44" s="200">
         <f ca="1">'April 2028 - June 2028'!E190</f>
-        <v>35052.78</v>
+        <v>35095.32</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -36721,7 +36718,7 @@
       </c>
       <c r="J45" s="200">
         <f ca="1">'July 2028 - September 2028'!E136</f>
-        <v>35858.78</v>
+        <v>35901.32</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -36741,7 +36738,7 @@
       </c>
       <c r="J46" s="200">
         <f ca="1">'July 2028 - September 2028'!E163</f>
-        <v>36725.78</v>
+        <v>36768.32</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -36766,7 +36763,7 @@
       </c>
       <c r="J47" s="200">
         <f ca="1">'July 2028 - September 2028'!E190</f>
-        <v>37481.78</v>
+        <v>37524.32</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -36789,7 +36786,7 @@
       </c>
       <c r="J48" s="200">
         <f ca="1">'October 2028 - December 2028'!E136</f>
-        <v>38508.78</v>
+        <v>38551.32</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -36808,7 +36805,7 @@
       </c>
       <c r="J49" s="200">
         <f ca="1">'October 2028 - December 2028'!E163</f>
-        <v>39104.78</v>
+        <v>39147.32</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -36827,13 +36824,13 @@
       </c>
       <c r="J50" s="196">
         <f ca="1">'October 2028 - December 2028'!E190</f>
-        <v>40131.78</v>
+        <v>40174.32</v>
       </c>
     </row>
     <row r="51" ht="41.1" customHeight="1" spans="1:7">
-      <c r="A51" s="172"/>
-      <c r="B51" s="173"/>
-      <c r="C51" s="173"/>
+      <c r="A51" s="173"/>
+      <c r="B51" s="174"/>
+      <c r="C51" s="174"/>
       <c r="D51" s="21"/>
       <c r="E51" s="21"/>
       <c r="F51" s="191">
@@ -36842,7 +36839,7 @@
       <c r="G51" s="44"/>
     </row>
     <row r="52" ht="24.75" customHeight="1" spans="1:7">
-      <c r="A52" s="174"/>
+      <c r="A52" s="175"/>
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
       <c r="D52" s="20"/>
@@ -36864,9 +36861,9 @@
       <c r="G53" s="44"/>
     </row>
     <row r="54" ht="24.75" customHeight="1" spans="1:7">
-      <c r="A54" s="168"/>
-      <c r="B54" s="169"/>
-      <c r="C54" s="170"/>
+      <c r="A54" s="169"/>
+      <c r="B54" s="170"/>
+      <c r="C54" s="171"/>
       <c r="D54" s="28" t="s">
         <v>51</v>
       </c>
@@ -36879,37 +36876,37 @@
     </row>
     <row r="55" ht="24.75" customHeight="1"/>
     <row r="58" ht="20.4" spans="1:3">
-      <c r="A58" s="175" t="str">
+      <c r="A58" s="176" t="str">
         <f>"Fixed Expense For the Year "&amp;TEXT(Main!B3,"mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,3)-1,"mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*3+2),"mmmm yyyy"))</f>
         <v>Fixed Expense For the Year January 2025 - April 2025</v>
       </c>
-      <c r="B58" s="176"/>
-      <c r="C58" s="177"/>
+      <c r="B58" s="177"/>
+      <c r="C58" s="178"/>
     </row>
     <row r="59" ht="21" spans="1:3">
-      <c r="A59" s="178" t="s">
+      <c r="A59" s="179" t="s">
         <v>48</v>
       </c>
-      <c r="B59" s="178" t="s">
+      <c r="B59" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="C59" s="179" t="s">
+      <c r="C59" s="180" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="180" t="s">
+      <c r="A60" s="181" t="s">
         <v>54</v>
       </c>
-      <c r="B60" s="181"/>
-      <c r="C60" s="182"/>
+      <c r="B60" s="182"/>
+      <c r="C60" s="183"/>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="B61" s="183"/>
-      <c r="C61" s="184">
+      <c r="B61" s="184"/>
+      <c r="C61" s="37">
         <v>78</v>
       </c>
     </row>
@@ -36917,8 +36914,8 @@
       <c r="A62" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="B62" s="183"/>
-      <c r="C62" s="184">
+      <c r="B62" s="184"/>
+      <c r="C62" s="37">
         <v>149</v>
       </c>
     </row>
@@ -36926,8 +36923,8 @@
       <c r="A63" s="185" t="s">
         <v>57</v>
       </c>
-      <c r="B63" s="183"/>
-      <c r="C63" s="184">
+      <c r="B63" s="184"/>
+      <c r="C63" s="37">
         <v>0</v>
       </c>
     </row>
@@ -36936,7 +36933,7 @@
         <v>58</v>
       </c>
       <c r="B64" s="186"/>
-      <c r="C64" s="184">
+      <c r="C64" s="37">
         <v>0</v>
       </c>
     </row>
@@ -36944,28 +36941,28 @@
       <c r="A65" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B65" s="183"/>
+      <c r="B65" s="184"/>
       <c r="C65" s="37">
         <v>50</v>
       </c>
     </row>
     <row r="66" ht="13" customHeight="1" spans="1:3">
       <c r="A66" s="51"/>
-      <c r="B66" s="183"/>
+      <c r="B66" s="184"/>
       <c r="C66" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="51"/>
-      <c r="B67" s="183"/>
+      <c r="B67" s="184"/>
       <c r="C67" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="51"/>
-      <c r="B68" s="183"/>
+      <c r="B68" s="184"/>
       <c r="C68" s="37">
         <v>0</v>
       </c>
@@ -36981,71 +36978,71 @@
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="180" t="s">
+      <c r="A70" s="181" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="181"/>
-      <c r="C70" s="182"/>
+      <c r="B70" s="182"/>
+      <c r="C70" s="183"/>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="51"/>
-      <c r="B71" s="183"/>
+      <c r="B71" s="184"/>
       <c r="C71" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="51"/>
-      <c r="B72" s="183"/>
+      <c r="B72" s="184"/>
       <c r="C72" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="51"/>
-      <c r="B73" s="183"/>
+      <c r="B73" s="184"/>
       <c r="C73" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="51"/>
-      <c r="B74" s="183"/>
+      <c r="B74" s="184"/>
       <c r="C74" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="51"/>
-      <c r="B75" s="183"/>
+      <c r="B75" s="184"/>
       <c r="C75" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="51"/>
-      <c r="B76" s="183"/>
+      <c r="B76" s="184"/>
       <c r="C76" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="51"/>
-      <c r="B77" s="183"/>
+      <c r="B77" s="184"/>
       <c r="C77" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="51"/>
-      <c r="B78" s="183"/>
+      <c r="B78" s="184"/>
       <c r="C78" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="51"/>
-      <c r="B79" s="183"/>
+      <c r="B79" s="184"/>
       <c r="C79" s="37">
         <v>0</v>
       </c>
@@ -37061,11 +37058,11 @@
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="180" t="s">
+      <c r="A81" s="181" t="s">
         <v>62</v>
       </c>
-      <c r="B81" s="181"/>
-      <c r="C81" s="182"/>
+      <c r="B81" s="182"/>
+      <c r="C81" s="183"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="51" t="s">
@@ -37082,7 +37079,7 @@
       <c r="A83" s="209" t="s">
         <v>65</v>
       </c>
-      <c r="B83" s="183" t="s">
+      <c r="B83" s="184" t="s">
         <v>66</v>
       </c>
       <c r="C83" s="37">
@@ -37091,35 +37088,35 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="52"/>
-      <c r="B84" s="183"/>
+      <c r="B84" s="184"/>
       <c r="C84" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="51"/>
-      <c r="B85" s="183"/>
+      <c r="B85" s="184"/>
       <c r="C85" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="51"/>
-      <c r="B86" s="183"/>
+      <c r="B86" s="184"/>
       <c r="C86" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="51"/>
-      <c r="B87" s="183"/>
+      <c r="B87" s="184"/>
       <c r="C87" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="51"/>
-      <c r="B88" s="183"/>
+      <c r="B88" s="184"/>
       <c r="C88" s="37">
         <v>0</v>
       </c>
@@ -37135,11 +37132,11 @@
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="180" t="s">
+      <c r="A90" s="181" t="s">
         <v>67</v>
       </c>
-      <c r="B90" s="181"/>
-      <c r="C90" s="182"/>
+      <c r="B90" s="182"/>
+      <c r="C90" s="183"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="210" t="s">
@@ -37152,49 +37149,49 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="52"/>
-      <c r="B92" s="183"/>
+      <c r="B92" s="184"/>
       <c r="C92" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="93" ht="20.25" customHeight="1" spans="1:3">
       <c r="A93" s="52"/>
-      <c r="B93" s="183"/>
+      <c r="B93" s="184"/>
       <c r="C93" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1" spans="1:3">
       <c r="A94" s="51"/>
-      <c r="B94" s="183"/>
+      <c r="B94" s="184"/>
       <c r="C94" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="51"/>
-      <c r="B95" s="183"/>
+      <c r="B95" s="184"/>
       <c r="C95" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="51"/>
-      <c r="B96" s="183"/>
+      <c r="B96" s="184"/>
       <c r="C96" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="51"/>
-      <c r="B97" s="183"/>
+      <c r="B97" s="184"/>
       <c r="C97" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="51"/>
-      <c r="B98" s="183"/>
+      <c r="B98" s="184"/>
       <c r="C98" s="37">
         <v>0</v>
       </c>
@@ -37210,11 +37207,11 @@
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="180" t="s">
+      <c r="A100" s="181" t="s">
         <v>69</v>
       </c>
-      <c r="B100" s="181"/>
-      <c r="C100" s="182"/>
+      <c r="B100" s="182"/>
+      <c r="C100" s="183"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="51" t="s">
@@ -37260,7 +37257,7 @@
       <c r="A105" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="B105" s="183" t="s">
+      <c r="B105" s="184" t="s">
         <v>77</v>
       </c>
       <c r="C105" s="213">
@@ -37269,21 +37266,21 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="51"/>
-      <c r="B106" s="183"/>
+      <c r="B106" s="184"/>
       <c r="C106" s="213">
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="51"/>
-      <c r="B107" s="183"/>
+      <c r="B107" s="184"/>
       <c r="C107" s="213">
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="51"/>
-      <c r="B108" s="183"/>
+      <c r="B108" s="184"/>
       <c r="C108" s="213">
         <v>0</v>
       </c>
@@ -37309,11 +37306,11 @@
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="180" t="s">
+      <c r="A111" s="181" t="s">
         <v>79</v>
       </c>
-      <c r="B111" s="181"/>
-      <c r="C111" s="182"/>
+      <c r="B111" s="182"/>
+      <c r="C111" s="183"/>
     </row>
     <row r="112" spans="1:8">
       <c r="A112" s="214" t="s">
@@ -37333,7 +37330,7 @@
       <c r="A113" s="214" t="s">
         <v>81</v>
       </c>
-      <c r="B113" s="183"/>
+      <c r="B113" s="184"/>
       <c r="C113" s="217">
         <v>0</v>
       </c>
@@ -37347,7 +37344,7 @@
       <c r="A114" s="214" t="s">
         <v>82</v>
       </c>
-      <c r="B114" s="183"/>
+      <c r="B114" s="184"/>
       <c r="C114" s="218">
         <v>0</v>
       </c>
@@ -37361,7 +37358,7 @@
       <c r="A115" s="219" t="s">
         <v>83</v>
       </c>
-      <c r="B115" s="183"/>
+      <c r="B115" s="184"/>
       <c r="C115" s="218">
         <v>0</v>
       </c>
@@ -37375,7 +37372,7 @@
       <c r="A116" s="219" t="s">
         <v>84</v>
       </c>
-      <c r="B116" s="183"/>
+      <c r="B116" s="184"/>
       <c r="C116" s="220">
         <v>326149.51</v>
       </c>
@@ -37389,7 +37386,7 @@
       <c r="A117" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="B117" s="183"/>
+      <c r="B117" s="184"/>
       <c r="C117" s="37">
         <v>1083</v>
       </c>
@@ -37399,13 +37396,13 @@
       <c r="G117" s="14"/>
       <c r="H117" s="14"/>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" ht="34" spans="1:8">
       <c r="A118" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="B118" s="183"/>
+      <c r="B118" s="184"/>
       <c r="C118" s="37">
-        <v>150.9</v>
+        <v>964.91</v>
       </c>
       <c r="D118" s="14"/>
       <c r="E118" s="14"/>
@@ -37415,7 +37412,7 @@
     </row>
     <row r="119" spans="1:8">
       <c r="A119" s="51"/>
-      <c r="B119" s="183"/>
+      <c r="B119" s="184"/>
       <c r="C119" s="37">
         <v>0</v>
       </c>
@@ -37427,7 +37424,7 @@
     </row>
     <row r="120" spans="1:8">
       <c r="A120" s="51"/>
-      <c r="B120" s="183"/>
+      <c r="B120" s="184"/>
       <c r="C120" s="37">
         <v>0</v>
       </c>
@@ -37439,7 +37436,7 @@
     </row>
     <row r="121" spans="1:8">
       <c r="A121" s="51"/>
-      <c r="B121" s="183"/>
+      <c r="B121" s="184"/>
       <c r="C121" s="37">
         <v>0</v>
       </c>
@@ -37456,7 +37453,7 @@
       </c>
       <c r="C122" s="213">
         <f>SUM(C112:C121)</f>
-        <v>333923.41</v>
+        <v>334737.42</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -37466,7 +37463,7 @@
       </c>
       <c r="C123" s="37">
         <f>C122+C110</f>
-        <v>334323.41</v>
+        <v>335137.42</v>
       </c>
     </row>
     <row r="124" spans="5:5">
@@ -37643,7 +37640,7 @@
       <c r="A142" s="63"/>
       <c r="B142" s="64"/>
       <c r="C142" s="114"/>
-      <c r="D142" s="148"/>
+      <c r="D142" s="149"/>
       <c r="E142" s="88">
         <v>0</v>
       </c>
@@ -37780,7 +37777,7 @@
       <c r="A159" s="63"/>
       <c r="B159" s="64"/>
       <c r="C159" s="114"/>
-      <c r="D159" s="148"/>
+      <c r="D159" s="149"/>
       <c r="E159" s="87">
         <v>0</v>
       </c>
@@ -38691,8 +38688,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="F179" sqref="F179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -38729,7 +38726,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -38743,7 +38740,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1188.78</v>
+        <v>1231.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -38757,7 +38754,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1652.56</v>
+        <v>1537.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -38773,7 +38770,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -38846,7 +38843,7 @@
       <c r="D10" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="140"/>
+      <c r="E10" s="141"/>
       <c r="F10" s="43">
         <v>0</v>
       </c>
@@ -38871,7 +38868,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="48"/>
     </row>
-    <row r="12" ht="64" customHeight="1" spans="1:9">
+    <row r="12" ht="86" customHeight="1" spans="1:9">
       <c r="A12" s="132"/>
       <c r="B12" s="97" t="s">
         <v>80</v>
@@ -38880,9 +38877,9 @@
       <c r="D12" s="97" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="141"/>
+      <c r="E12" s="142"/>
       <c r="F12" s="43">
-        <v>820.9</v>
+        <v>670</v>
       </c>
       <c r="G12" s="44"/>
       <c r="H12" s="14"/>
@@ -38894,7 +38891,7 @@
       <c r="C13" s="98"/>
       <c r="D13" s="97"/>
       <c r="E13" s="115"/>
-      <c r="F13" s="142">
+      <c r="F13" s="143">
         <v>0</v>
       </c>
       <c r="G13" s="44"/>
@@ -38937,7 +38934,7 @@
       <c r="E16" s="45"/>
       <c r="F16" s="46">
         <f>SUM(F10:G15)</f>
-        <v>1220.9</v>
+        <v>1070</v>
       </c>
       <c r="G16" s="47"/>
       <c r="H16" s="14"/>
@@ -39018,21 +39015,21 @@
       <c r="D22" s="133" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="140"/>
-      <c r="F22" s="143">
+      <c r="E22" s="141"/>
+      <c r="F22" s="144">
         <v>3483</v>
       </c>
-      <c r="G22" s="144"/>
+      <c r="G22" s="145"/>
       <c r="H22" s="14"/>
       <c r="I22" s="48"/>
     </row>
-    <row r="23" ht="26.25" customHeight="1" spans="1:9">
+    <row r="23" ht="139" customHeight="1" spans="1:9">
       <c r="A23" s="132"/>
       <c r="B23" s="97" t="s">
         <v>80</v>
       </c>
       <c r="C23" s="98"/>
-      <c r="D23" s="99" t="s">
+      <c r="D23" s="137" t="s">
         <v>101</v>
       </c>
       <c r="E23" s="100"/>
@@ -39043,7 +39040,7 @@
       <c r="H23" s="14"/>
       <c r="I23" s="48"/>
     </row>
-    <row r="24" ht="45" customHeight="1" spans="1:9">
+    <row r="24" ht="48" customHeight="1" spans="1:9">
       <c r="A24" s="132"/>
       <c r="B24" s="97" t="s">
         <v>102</v>
@@ -39052,7 +39049,7 @@
       <c r="D24" s="97" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="141"/>
+      <c r="E24" s="142"/>
       <c r="F24" s="104">
         <v>204</v>
       </c>
@@ -39069,7 +39066,7 @@
       <c r="D25" s="97" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="141"/>
+      <c r="E25" s="142"/>
       <c r="F25" s="43">
         <v>69.99</v>
       </c>
@@ -39077,7 +39074,7 @@
       <c r="H25" s="14"/>
       <c r="I25" s="48"/>
     </row>
-    <row r="26" ht="48" customHeight="1" spans="1:9">
+    <row r="26" ht="79" customHeight="1" spans="1:9">
       <c r="A26" s="132"/>
       <c r="B26" s="97" t="s">
         <v>106</v>
@@ -39087,7 +39084,7 @@
         <v>107</v>
       </c>
       <c r="E26" s="115"/>
-      <c r="F26" s="142">
+      <c r="F26" s="143">
         <v>0</v>
       </c>
       <c r="G26" s="44"/>
@@ -39096,14 +39093,14 @@
     </row>
     <row r="27" ht="39" customHeight="1" spans="1:9">
       <c r="A27" s="132"/>
-      <c r="B27" s="137" t="s">
+      <c r="B27" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="138"/>
-      <c r="D27" s="137" t="s">
+      <c r="C27" s="139"/>
+      <c r="D27" s="138" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="145"/>
+      <c r="E27" s="146"/>
       <c r="F27" s="43">
         <v>3</v>
       </c>
@@ -39200,11 +39197,11 @@
       </c>
       <c r="C34" s="134"/>
       <c r="D34" s="135"/>
-      <c r="E34" s="140"/>
-      <c r="F34" s="143">
+      <c r="E34" s="141"/>
+      <c r="F34" s="144">
         <v>2435</v>
       </c>
-      <c r="G34" s="144"/>
+      <c r="G34" s="145"/>
       <c r="H34" s="14"/>
       <c r="I34" s="48"/>
     </row>
@@ -39217,7 +39214,7 @@
       <c r="D35" s="123" t="s">
         <v>111</v>
       </c>
-      <c r="E35" s="146"/>
+      <c r="E35" s="147"/>
       <c r="F35" s="7">
         <v>50</v>
       </c>
@@ -39234,7 +39231,7 @@
       <c r="D36" s="123" t="s">
         <v>112</v>
       </c>
-      <c r="E36" s="146"/>
+      <c r="E36" s="147"/>
       <c r="F36" s="7">
         <v>19.99</v>
       </c>
@@ -39242,16 +39239,12 @@
       <c r="H36" s="14"/>
       <c r="I36" s="49"/>
     </row>
-    <row r="37" ht="45" customHeight="1" spans="1:9">
+    <row r="37" ht="25" customHeight="1" spans="1:9">
       <c r="A37" s="132"/>
-      <c r="B37" s="97" t="s">
-        <v>113</v>
-      </c>
+      <c r="B37" s="97"/>
       <c r="C37" s="98"/>
-      <c r="D37" s="97" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" s="146"/>
+      <c r="D37" s="97"/>
+      <c r="E37" s="147"/>
       <c r="F37" s="7">
         <v>0</v>
       </c>
@@ -39264,7 +39257,7 @@
       <c r="B38" s="97"/>
       <c r="C38" s="98"/>
       <c r="D38" s="123"/>
-      <c r="E38" s="141"/>
+      <c r="E38" s="142"/>
       <c r="F38" s="104">
         <v>0</v>
       </c>
@@ -39388,7 +39381,7 @@
         <f ca="1" t="array" ref="B47">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B61"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B61")))</f>
         <v/>
       </c>
-      <c r="C47" s="139">
+      <c r="C47" s="140">
         <v>78</v>
       </c>
       <c r="D47" s="14"/>
@@ -39407,7 +39400,7 @@
         <f ca="1" t="array" ref="B48">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B62"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B62")))</f>
         <v/>
       </c>
-      <c r="C48" s="139">
+      <c r="C48" s="140">
         <v>149</v>
       </c>
       <c r="D48" s="14"/>
@@ -39426,7 +39419,7 @@
         <f ca="1" t="array" ref="B49">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B63"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B63")))</f>
         <v/>
       </c>
-      <c r="C49" s="139">
+      <c r="C49" s="140">
         <v>0</v>
       </c>
       <c r="D49" s="14"/>
@@ -39445,7 +39438,7 @@
         <f ca="1" t="array" ref="B50">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B64"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B64")))</f>
         <v/>
       </c>
-      <c r="C50" s="139">
+      <c r="C50" s="140">
         <v>0</v>
       </c>
       <c r="D50" s="14"/>
@@ -40398,7 +40391,7 @@
         <v>-326149.51</v>
       </c>
       <c r="D102" s="14"/>
-      <c r="E102" s="147"/>
+      <c r="E102" s="148"/>
       <c r="F102" s="14"/>
       <c r="G102" s="14"/>
       <c r="H102" s="14"/>
@@ -40427,7 +40420,7 @@
     <row r="104" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -40435,7 +40428,7 @@
       </c>
       <c r="C104" s="106" cm="1">
         <f ca="1" t="array" ref="C104">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E137")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E164")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E191")))+SUM(E124+E151+E178))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C118")</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -40511,7 +40504,7 @@
       </c>
       <c r="C108" s="106">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -40527,7 +40520,7 @@
       </c>
       <c r="C109" s="106">
         <f ca="1">C108-C96</f>
-        <v>-333622.5</v>
+        <v>-334150.01</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -40790,7 +40783,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -40805,7 +40798,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="73" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -40819,12 +40812,10 @@
     <row r="131" ht="24.75" customHeight="1" spans="1:9">
       <c r="A131" s="63"/>
       <c r="B131" s="64"/>
-      <c r="C131" s="74" t="s">
-        <v>117</v>
-      </c>
+      <c r="C131" s="74"/>
       <c r="D131" s="74"/>
       <c r="E131" s="87">
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="F131" s="14"/>
       <c r="G131" s="14"/>
@@ -41013,7 +41004,7 @@
       <c r="A145" s="63"/>
       <c r="B145" s="64"/>
       <c r="C145" s="65" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D145" s="66"/>
       <c r="E145" s="37">
@@ -41089,15 +41080,15 @@
       <c r="H150" s="14"/>
       <c r="I150" s="48"/>
     </row>
-    <row r="151" ht="27" customHeight="1" spans="1:9">
+    <row r="151" ht="119" customHeight="1" spans="1:9">
       <c r="A151" s="63"/>
       <c r="B151" s="64"/>
       <c r="C151" s="114" t="s">
-        <v>119</v>
-      </c>
-      <c r="D151" s="148"/>
+        <v>116</v>
+      </c>
+      <c r="D151" s="149"/>
       <c r="E151" s="37">
-        <v>150.9</v>
+        <v>437.4</v>
       </c>
       <c r="F151" s="14"/>
       <c r="G151" s="14"/>
@@ -41160,7 +41151,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -41175,7 +41166,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="73" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -41186,11 +41177,11 @@
       <c r="H157" s="14"/>
       <c r="I157" s="48"/>
     </row>
-    <row r="158" ht="118" customHeight="1" spans="1:9">
+    <row r="158" ht="136" customHeight="1" spans="1:9">
       <c r="A158" s="63"/>
       <c r="B158" s="64"/>
       <c r="C158" s="73" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D158" s="74"/>
       <c r="E158" s="87">
@@ -41201,41 +41192,41 @@
       <c r="H158" s="14"/>
       <c r="I158" s="48"/>
     </row>
-    <row r="159" ht="282" customHeight="1" spans="1:9">
+    <row r="159" ht="324" customHeight="1" spans="1:9">
       <c r="A159" s="63"/>
       <c r="B159" s="64"/>
       <c r="C159" s="73" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D159" s="74"/>
       <c r="E159" s="87">
-        <v>428.5</v>
+        <v>505.5</v>
       </c>
       <c r="F159" s="14"/>
       <c r="G159" s="14"/>
       <c r="H159" s="14"/>
       <c r="I159" s="48"/>
     </row>
-    <row r="160" ht="281" customHeight="1" spans="1:9">
+    <row r="160" ht="299" customHeight="1" spans="1:9">
       <c r="A160" s="63"/>
       <c r="B160" s="64"/>
       <c r="C160" s="73" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D160" s="125"/>
       <c r="E160" s="87">
-        <v>622.24</v>
+        <v>416.2</v>
       </c>
       <c r="F160" s="14"/>
       <c r="G160" s="14"/>
       <c r="H160" s="14"/>
       <c r="I160" s="48"/>
     </row>
-    <row r="161" ht="24" customHeight="1" spans="1:9">
+    <row r="161" ht="25" customHeight="1" spans="1:9">
       <c r="A161" s="75"/>
       <c r="B161" s="76"/>
-      <c r="C161" s="65"/>
-      <c r="D161" s="66"/>
+      <c r="C161" s="114"/>
+      <c r="D161" s="149"/>
       <c r="E161" s="88">
         <v>0</v>
       </c>
@@ -41269,7 +41260,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -41353,14 +41344,14 @@
     </row>
     <row r="170" ht="24.75" customHeight="1" spans="1:9">
       <c r="A170" s="56" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -41386,7 +41377,7 @@
       <c r="A172" s="63"/>
       <c r="B172" s="64"/>
       <c r="C172" s="74" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
@@ -41453,7 +41444,7 @@
       <c r="A177" s="63"/>
       <c r="B177" s="64"/>
       <c r="C177" s="114"/>
-      <c r="D177" s="148"/>
+      <c r="D177" s="149"/>
       <c r="E177" s="37">
         <v>0</v>
       </c>
@@ -41462,11 +41453,13 @@
       <c r="H177" s="14"/>
       <c r="I177" s="48"/>
     </row>
-    <row r="178" ht="24.75" customHeight="1" spans="1:9">
+    <row r="178" ht="47" customHeight="1" spans="1:9">
       <c r="A178" s="63"/>
       <c r="B178" s="64"/>
-      <c r="C178" s="114"/>
-      <c r="D178" s="148"/>
+      <c r="C178" s="114" t="s">
+        <v>124</v>
+      </c>
+      <c r="D178" s="149"/>
       <c r="E178" s="37">
         <v>0</v>
       </c>
@@ -41527,15 +41520,15 @@
       <c r="H182" s="14"/>
       <c r="I182" s="48"/>
     </row>
-    <row r="183" ht="62" customHeight="1" spans="1:9">
+    <row r="183" ht="50" customHeight="1" spans="1:9">
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
-        <v>960</v>
+        <v>760</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -41546,7 +41539,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -41557,12 +41550,10 @@
       <c r="H184" s="14"/>
       <c r="I184" s="48"/>
     </row>
-    <row r="185" ht="46" customHeight="1" spans="1:9">
+    <row r="185" ht="25" customHeight="1" spans="1:9">
       <c r="A185" s="63"/>
       <c r="B185" s="64"/>
-      <c r="C185" s="73" t="s">
-        <v>129</v>
-      </c>
+      <c r="C185" s="73"/>
       <c r="D185" s="73"/>
       <c r="E185" s="87">
         <v>0</v>
@@ -41601,8 +41592,8 @@
     <row r="188" ht="24.75" customHeight="1" spans="1:9">
       <c r="A188" s="75"/>
       <c r="B188" s="76"/>
-      <c r="C188" s="149"/>
-      <c r="D188" s="150"/>
+      <c r="C188" s="150"/>
+      <c r="D188" s="151"/>
       <c r="E188" s="87">
         <v>0</v>
       </c>
@@ -41636,7 +41627,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1188.78</v>
+        <v>1231.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -41656,7 +41647,7 @@
     </row>
     <row r="193" s="41" customFormat="1" ht="24.75" customHeight="1"/>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -42125,7 +42116,7 @@
   <sheetPr/>
   <dimension ref="A1:I192"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A111" workbookViewId="0">
       <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
@@ -42160,7 +42151,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -42174,7 +42165,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4128.78</v>
+        <v>4171.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -42188,7 +42179,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4592.56</v>
+        <v>4477.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -42204,7 +42195,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -43815,7 +43806,7 @@
     <row r="104" ht="30" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -43823,7 +43814,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -43899,7 +43890,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -43915,7 +43906,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -44009,7 +44000,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="89" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!E190")</f>
-        <v>1188.78</v>
+        <v>1231.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -44035,7 +44026,7 @@
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
       <c r="C118" s="74" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D118" s="74"/>
       <c r="E118" s="37">
@@ -44180,7 +44171,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -44195,7 +44186,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -44283,7 +44274,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>2215.78</v>
+        <v>2258.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -44375,7 +44366,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>2215.78</v>
+        <v>2258.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -44401,7 +44392,7 @@
       <c r="A145" s="63"/>
       <c r="B145" s="64"/>
       <c r="C145" s="74" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D145" s="74"/>
       <c r="E145" s="37">
@@ -44546,7 +44537,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -44561,7 +44552,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -44649,7 +44640,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3101.78</v>
+        <v>3144.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -44741,7 +44732,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>3101.78</v>
+        <v>3144.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -44767,7 +44758,7 @@
       <c r="A172" s="63"/>
       <c r="B172" s="64"/>
       <c r="C172" s="74" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
@@ -44912,7 +44903,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -44927,7 +44918,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -45015,7 +45006,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4128.78</v>
+        <v>4171.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -45580,7 +45571,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -45596,7 +45587,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>6847.78</v>
+        <v>6890.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -45612,7 +45603,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>7311.56</v>
+        <v>7196.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -45628,7 +45619,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -47239,7 +47230,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -47247,7 +47238,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -47323,7 +47314,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -47339,7 +47330,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -47433,7 +47424,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!E190")</f>
-        <v>4128.78</v>
+        <v>4171.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -47459,7 +47450,7 @@
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
       <c r="C118" s="74" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D118" s="74"/>
       <c r="E118" s="37">
@@ -47604,7 +47595,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -47619,7 +47610,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -47707,7 +47698,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5064.78</v>
+        <v>5107.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -47799,7 +47790,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>5064.78</v>
+        <v>5107.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -47825,7 +47816,7 @@
       <c r="A145" s="63"/>
       <c r="B145" s="64"/>
       <c r="C145" s="74" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D145" s="74"/>
       <c r="E145" s="37">
@@ -47892,7 +47883,7 @@
       <c r="A150" s="63"/>
       <c r="B150" s="64"/>
       <c r="C150" s="65" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D150" s="66"/>
       <c r="E150" s="37">
@@ -47972,7 +47963,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -47987,7 +47978,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -48075,7 +48066,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>6041.78</v>
+        <v>6084.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -48167,7 +48158,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>6041.78</v>
+        <v>6084.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -48193,7 +48184,7 @@
       <c r="A172" s="63"/>
       <c r="B172" s="64"/>
       <c r="C172" s="74" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
@@ -48260,7 +48251,7 @@
       <c r="A177" s="63"/>
       <c r="B177" s="64"/>
       <c r="C177" s="65" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D177" s="66"/>
       <c r="E177" s="37">
@@ -48340,7 +48331,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -48355,7 +48346,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -48443,7 +48434,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6847.78</v>
+        <v>6890.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -48982,8 +48973,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -49018,7 +49009,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -49034,7 +49025,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>9497.78</v>
+        <v>9540.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -49050,7 +49041,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>9961.56</v>
+        <v>9846.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -49066,7 +49057,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -50677,7 +50668,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -50685,7 +50676,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -50761,7 +50752,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -50777,7 +50768,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -50871,7 +50862,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>6847.78</v>
+        <v>6890.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -50897,7 +50888,7 @@
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
       <c r="C118" s="74" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D118" s="74"/>
       <c r="E118" s="87">
@@ -50964,7 +50955,7 @@
       <c r="A123" s="63"/>
       <c r="B123" s="64"/>
       <c r="C123" s="65" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D123" s="66"/>
       <c r="E123" s="37">
@@ -51044,7 +51035,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -51059,7 +51050,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -51147,7 +51138,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>7874.78</v>
+        <v>7917.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -51239,7 +51230,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>7874.78</v>
+        <v>7917.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -51408,7 +51399,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -51423,7 +51414,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -51511,7 +51502,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>8470.78</v>
+        <v>8513.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -51603,7 +51594,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>8470.78</v>
+        <v>8513.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -51772,7 +51763,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -51787,7 +51778,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -51875,7 +51866,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>9497.78</v>
+        <v>9540.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -52408,7 +52399,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -52424,7 +52415,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>12859.78</v>
+        <v>12902.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -52440,7 +52431,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>13323.56</v>
+        <v>13208.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -52456,7 +52447,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -52708,7 +52699,7 @@
       </c>
       <c r="C23" s="98"/>
       <c r="D23" s="99" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E23" s="100"/>
       <c r="F23" s="7">
@@ -54071,7 +54062,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -54079,7 +54070,7 @@
       </c>
       <c r="C104" s="106" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -54155,7 +54146,7 @@
       </c>
       <c r="C108" s="106">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -54171,7 +54162,7 @@
       </c>
       <c r="C109" s="106">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -54265,7 +54256,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>9497.78</v>
+        <v>9540.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -54434,7 +54425,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -54449,7 +54440,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -54537,7 +54528,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>10253.78</v>
+        <v>10296.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -54629,7 +54620,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>10253.78</v>
+        <v>10296.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -54798,7 +54789,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -54813,7 +54804,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -54901,7 +54892,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>12203.78</v>
+        <v>12246.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -54993,7 +54984,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>12203.78</v>
+        <v>12246.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -55162,7 +55153,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -55177,7 +55168,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -55265,7 +55256,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>12859.78</v>
+        <v>12902.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -55795,7 +55786,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>463.78</v>
+        <v>306.32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -55811,7 +55802,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>15509.78</v>
+        <v>15552.32</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -55827,7 +55818,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>15973.56</v>
+        <v>15858.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55843,7 +55834,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -55926,7 +55917,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="101" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -57456,7 +57447,7 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A118")))</f>
-        <v>Mother Amazon Books</v>
+        <v>Mother Borrowed Credit Card</v>
       </c>
       <c r="B104" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B104">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B118")))</f>
@@ -57464,7 +57455,7 @@
       </c>
       <c r="C104" s="106" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>0</v>
+        <v>-527.51</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -57540,7 +57531,7 @@
       </c>
       <c r="C108" s="106">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333202.51</v>
+        <v>-333730.02</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -57556,7 +57547,7 @@
       </c>
       <c r="C109" s="106">
         <f ca="1">C108-C96</f>
-        <v>-333541.51</v>
+        <v>-334069.02</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -57650,7 +57641,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>12859.78</v>
+        <v>12902.32</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -57819,7 +57810,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -57834,7 +57825,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -57922,7 +57913,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>13886.78</v>
+        <v>13929.32</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -58014,7 +58005,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>13886.78</v>
+        <v>13929.32</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -58183,7 +58174,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -58198,7 +58189,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -58286,7 +58277,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14482.78</v>
+        <v>14525.32</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -58378,7 +58369,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>14482.78</v>
+        <v>14525.32</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -58547,7 +58538,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -58562,7 +58553,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -58650,7 +58641,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>15509.78</v>
+        <v>15552.32</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: Beginning of the Forecast Month July.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21480" activeTab="3"/>
+    <workbookView windowHeight="21480"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -3136,7 +3136,7 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17781.32</v>
+        <v>18413.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -4965,7 +4965,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18087.64</v>
+        <v>20400.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -4981,7 +4981,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -6600,7 +6600,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -6676,7 +6676,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -6692,7 +6692,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -6786,7 +6786,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>15552.32</v>
+        <v>16184.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7058,7 +7058,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>16308.32</v>
+        <v>16940.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7150,7 +7150,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>16308.32</v>
+        <v>16940.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -7422,7 +7422,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17175.32</v>
+        <v>17807.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -7514,7 +7514,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>17175.32</v>
+        <v>17807.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -7786,7 +7786,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17781.32</v>
+        <v>18413.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -8302,7 +8302,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -8318,7 +8318,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>20431.32</v>
+        <v>21063.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -8334,7 +8334,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>20737.64</v>
+        <v>23050.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -8350,7 +8350,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -9969,7 +9969,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -10045,7 +10045,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -10061,7 +10061,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -10155,7 +10155,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>17781.32</v>
+        <v>18413.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -10427,7 +10427,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>18808.32</v>
+        <v>19440.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -10519,7 +10519,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>18808.32</v>
+        <v>19440.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -10791,7 +10791,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19404.32</v>
+        <v>20036.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -10883,7 +10883,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>19404.32</v>
+        <v>20036.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11155,7 +11155,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>20431.32</v>
+        <v>21063.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -11667,7 +11667,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -11683,7 +11683,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>24164.32</v>
+        <v>24796.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -11699,7 +11699,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>24470.64</v>
+        <v>26783.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -11715,7 +11715,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -13338,7 +13338,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -13414,7 +13414,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -13430,7 +13430,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -13524,7 +13524,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>20431.32</v>
+        <v>21063.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -13796,7 +13796,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>21458.32</v>
+        <v>22090.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -13888,7 +13888,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>21458.32</v>
+        <v>22090.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14160,7 +14160,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>23137.32</v>
+        <v>23769.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -14252,7 +14252,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>23137.32</v>
+        <v>23769.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -14524,7 +14524,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>24164.32</v>
+        <v>24796.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15042,7 +15042,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15058,7 +15058,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>26393.32</v>
+        <v>27025.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15074,7 +15074,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>26699.64</v>
+        <v>29012.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -15090,7 +15090,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -16709,7 +16709,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -16785,7 +16785,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -16801,7 +16801,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -16895,7 +16895,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>24164.32</v>
+        <v>24796.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -17167,7 +17167,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>24920.32</v>
+        <v>25552.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -17259,7 +17259,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>24920.32</v>
+        <v>25552.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -17531,7 +17531,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>25787.32</v>
+        <v>26419.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -17623,7 +17623,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>25787.32</v>
+        <v>26419.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -17895,7 +17895,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>26393.32</v>
+        <v>27025.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -18412,7 +18412,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -18428,7 +18428,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>29043.32</v>
+        <v>29675.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -18444,7 +18444,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>29349.64</v>
+        <v>31662.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -18460,7 +18460,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -20079,7 +20079,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -20155,7 +20155,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -20171,7 +20171,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -20265,7 +20265,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>26393.32</v>
+        <v>27025.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -20537,7 +20537,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>27420.32</v>
+        <v>28052.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -20629,7 +20629,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>27420.32</v>
+        <v>28052.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -20901,7 +20901,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>28016.32</v>
+        <v>28648.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -20993,7 +20993,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>28016.32</v>
+        <v>28648.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -21265,7 +21265,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>29043.32</v>
+        <v>29675.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -21775,7 +21775,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -21791,7 +21791,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>31362.32</v>
+        <v>31994.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -21807,7 +21807,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>31668.64</v>
+        <v>33981.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -21823,7 +21823,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -23442,7 +23442,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -23518,7 +23518,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -23534,7 +23534,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -23628,7 +23628,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>29043.32</v>
+        <v>29675.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -23900,7 +23900,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>29849.32</v>
+        <v>30481.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -23992,7 +23992,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>29849.32</v>
+        <v>30481.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -24264,7 +24264,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>30716.32</v>
+        <v>31348.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -24356,7 +24356,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>30716.32</v>
+        <v>31348.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -24628,7 +24628,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>31362.32</v>
+        <v>31994.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -25144,7 +25144,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -25160,7 +25160,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35095.32</v>
+        <v>35727.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -25176,7 +25176,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35401.64</v>
+        <v>37714.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -25192,7 +25192,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -26815,7 +26815,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -26891,7 +26891,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -26907,7 +26907,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -27001,7 +27001,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>31362.32</v>
+        <v>31994.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -27273,7 +27273,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>32389.32</v>
+        <v>33021.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -27365,7 +27365,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>32389.32</v>
+        <v>33021.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -27637,7 +27637,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>34068.32</v>
+        <v>34700.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -27729,7 +27729,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>34068.32</v>
+        <v>34700.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -28001,7 +28001,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35095.32</v>
+        <v>35727.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -28498,7 +28498,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -28514,7 +28514,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>37524.32</v>
+        <v>38156.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -28530,7 +28530,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>37830.64</v>
+        <v>40143.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28546,7 +28546,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -30164,7 +30164,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -30240,7 +30240,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -30256,7 +30256,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -30350,7 +30350,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>35095.32</v>
+        <v>35727.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -30622,7 +30622,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35901.32</v>
+        <v>36533.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -30714,7 +30714,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>35901.32</v>
+        <v>36533.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -30986,7 +30986,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>36768.32</v>
+        <v>37400.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -31078,7 +31078,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>36768.32</v>
+        <v>37400.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -31350,7 +31350,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>37524.32</v>
+        <v>38156.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -31854,7 +31854,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -31870,7 +31870,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>40174.32</v>
+        <v>40806.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -31886,7 +31886,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>40480.64</v>
+        <v>42793.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31902,7 +31902,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -33521,7 +33521,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -33597,7 +33597,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -33613,7 +33613,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -33707,7 +33707,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>37524.32</v>
+        <v>38156.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -33979,7 +33979,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>38551.32</v>
+        <v>39183.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -34071,7 +34071,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>38551.32</v>
+        <v>39183.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -34343,7 +34343,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>39147.32</v>
+        <v>39779.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -34435,7 +34435,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>39147.32</v>
+        <v>39779.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -34707,7 +34707,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>40174.32</v>
+        <v>40806.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -35709,8 +35709,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -35781,7 +35781,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="159">
-        <v>118.5</v>
+        <v>1798.99</v>
       </c>
       <c r="D3" s="160" t="s">
         <v>33</v>
@@ -35790,7 +35790,7 @@
         <v>34</v>
       </c>
       <c r="F3" s="187">
-        <v>256</v>
+        <v>118.5</v>
       </c>
       <c r="I3" s="195" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*1,"dd mmmm yyyy"))</f>
@@ -35838,7 +35838,7 @@
       </c>
       <c r="N4" s="196">
         <f ca="1">'April 2025 - June 2025'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="5" ht="35.25" customHeight="1" spans="1:14">
@@ -35870,7 +35870,7 @@
       </c>
       <c r="N5" s="196">
         <f ca="1">'July 2025 - September 2025'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="6" ht="35.25" customHeight="1" spans="1:14">
@@ -35902,7 +35902,7 @@
       </c>
       <c r="N6" s="196">
         <f ca="1">'October 2025 - December 2025'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="7" ht="35.25" customHeight="1" spans="1:14">
@@ -35918,7 +35918,7 @@
         <v>38</v>
       </c>
       <c r="F7" s="187">
-        <v>32.96</v>
+        <v>0</v>
       </c>
       <c r="I7" s="198" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,4),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*4)+4,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,5)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*5+4),"dd mmmm yyyy"))</f>
@@ -35934,7 +35934,7 @@
       </c>
       <c r="N7" s="196">
         <f ca="1">'January 2026 - March 2026'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="8" ht="45" customHeight="1" spans="1:14">
@@ -35959,7 +35959,7 @@
       </c>
       <c r="J8" s="196">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>1231.32</v>
+        <v>1863.81</v>
       </c>
       <c r="M8" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,15),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+15),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,18)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+17),"dd mmmm yyyy"))</f>
@@ -35967,7 +35967,7 @@
       </c>
       <c r="N8" s="196">
         <f ca="1">'April 2026 - June 2026'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="9" ht="39.75" customHeight="1" spans="1:14">
@@ -35991,7 +35991,7 @@
       </c>
       <c r="J9" s="196">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>2258.32</v>
+        <v>2890.81</v>
       </c>
       <c r="M9" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,18),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+18),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,21)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+20),"dd mmmm yyyy"))</f>
@@ -35999,7 +35999,7 @@
       </c>
       <c r="N9" s="205">
         <f ca="1">'July 2026 - September 2026'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="10" ht="35.25" customHeight="1" spans="1:14">
@@ -36023,7 +36023,7 @@
       </c>
       <c r="J10" s="196">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>3144.32</v>
+        <v>3776.81</v>
       </c>
       <c r="M10" s="206" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,21),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+21),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,24)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+23),"dd mmmm yyyy"))</f>
@@ -36031,7 +36031,7 @@
       </c>
       <c r="N10" s="196">
         <f ca="1">'October 2026 - December 2026'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="11" ht="35.25" customHeight="1" spans="1:14">
@@ -36056,7 +36056,7 @@
       </c>
       <c r="J11" s="196">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>4171.32</v>
+        <v>4803.81</v>
       </c>
       <c r="M11" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,24),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+24),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,27)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+26),"dd mmmm yyyy"))</f>
@@ -36064,7 +36064,7 @@
       </c>
       <c r="N11" s="200">
         <f ca="1">'January 2027 - March 2027'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="12" ht="35.25" customHeight="1" spans="1:14">
@@ -36080,7 +36080,7 @@
         <v>43</v>
       </c>
       <c r="F12" s="187">
-        <v>30.02</v>
+        <v>180.02</v>
       </c>
       <c r="I12" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,9),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*9)+9,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,10)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*10+9),"dd mmmm yyyy"))</f>
@@ -36088,7 +36088,7 @@
       </c>
       <c r="J12" s="196">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>5107.32</v>
+        <v>5739.81</v>
       </c>
       <c r="M12" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,27),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+27),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,30)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+29),"dd mmmm yyyy"))</f>
@@ -36096,7 +36096,7 @@
       </c>
       <c r="N12" s="200">
         <f ca="1">'April 2027 - June 2027'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="13" ht="35.25" customHeight="1" spans="1:14">
@@ -36120,7 +36120,7 @@
       </c>
       <c r="J13" s="196">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>6084.32</v>
+        <v>6716.81</v>
       </c>
       <c r="M13" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,30),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+30),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,33)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+32),"dd mmmm yyyy"))</f>
@@ -36128,7 +36128,7 @@
       </c>
       <c r="N13" s="200">
         <f ca="1">'July 2027 - September 2027'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="14" ht="35.25" customHeight="1" spans="1:14">
@@ -36152,7 +36152,7 @@
       </c>
       <c r="J14" s="200">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>6890.32</v>
+        <v>7522.81</v>
       </c>
       <c r="M14" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -36160,7 +36160,7 @@
       </c>
       <c r="N14" s="200">
         <f ca="1">'October 2027 - December 2027'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="15" ht="35.25" customHeight="1" spans="1:14">
@@ -36184,7 +36184,7 @@
       </c>
       <c r="J15" s="200">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>7917.32</v>
+        <v>8549.81</v>
       </c>
       <c r="M15" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -36192,7 +36192,7 @@
       </c>
       <c r="N15" s="200">
         <f ca="1">'January 2028 - March 2028'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="16" ht="35.25" customHeight="1" spans="1:14">
@@ -36202,7 +36202,7 @@
       </c>
       <c r="C16" s="165">
         <f>SUM(C3:C15)</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D16" s="166"/>
       <c r="E16" s="164" t="s">
@@ -36210,7 +36210,7 @@
       </c>
       <c r="F16" s="190">
         <f>SUM(F3:F15)</f>
-        <v>326.78</v>
+        <v>306.32</v>
       </c>
       <c r="I16" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -36218,7 +36218,7 @@
       </c>
       <c r="J16" s="200">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>8513.32</v>
+        <v>9145.81</v>
       </c>
       <c r="M16" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -36226,7 +36226,7 @@
       </c>
       <c r="N16" s="200">
         <f ca="1">'April 2028 - June 2028'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="17" ht="35.25" customHeight="1" spans="9:14">
@@ -36236,7 +36236,7 @@
       </c>
       <c r="J17" s="200">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>9540.32</v>
+        <v>10172.81</v>
       </c>
       <c r="M17" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -36244,7 +36244,7 @@
       </c>
       <c r="N17" s="200">
         <f ca="1">'July 2028 - September 2028'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="18" ht="35.25" customHeight="1" spans="9:14">
@@ -36254,7 +36254,7 @@
       </c>
       <c r="J18" s="200">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>10296.32</v>
+        <v>10928.81</v>
       </c>
       <c r="M18" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -36262,7 +36262,7 @@
       </c>
       <c r="N18" s="196">
         <f ca="1">'October 2028 - December 2028'!C5</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
     </row>
     <row r="19" ht="33" customHeight="1" spans="9:10">
@@ -36272,7 +36272,7 @@
       </c>
       <c r="J19" s="200">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>12246.32</v>
+        <v>12878.81</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -36282,7 +36282,7 @@
       </c>
       <c r="J20" s="200">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>12902.32</v>
+        <v>13534.81</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -36292,7 +36292,7 @@
       </c>
       <c r="J21" s="200">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>13929.32</v>
+        <v>14561.81</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -36312,7 +36312,7 @@
       </c>
       <c r="J22" s="200">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>14525.32</v>
+        <v>15157.81</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -36337,7 +36337,7 @@
       </c>
       <c r="J23" s="200">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>15552.32</v>
+        <v>16184.81</v>
       </c>
     </row>
     <row r="24" ht="33" customHeight="1" spans="1:10">
@@ -36356,7 +36356,7 @@
       </c>
       <c r="J24" s="200">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>16308.32</v>
+        <v>16940.81</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -36375,7 +36375,7 @@
       </c>
       <c r="J25" s="200">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>17175.32</v>
+        <v>17807.81</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -36394,7 +36394,7 @@
       </c>
       <c r="J26" s="200">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>17781.32</v>
+        <v>18413.81</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -36413,7 +36413,7 @@
       </c>
       <c r="J27" s="200">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>18808.32</v>
+        <v>19440.81</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -36432,7 +36432,7 @@
       </c>
       <c r="J28" s="200">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>19404.32</v>
+        <v>20036.81</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -36451,7 +36451,7 @@
       </c>
       <c r="J29" s="196">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>20431.32</v>
+        <v>21063.81</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -36473,7 +36473,7 @@
       </c>
       <c r="J30" s="202">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>21458.32</v>
+        <v>22090.81</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -36483,7 +36483,7 @@
       </c>
       <c r="J31" s="200">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>23137.32</v>
+        <v>23769.81</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -36493,7 +36493,7 @@
       </c>
       <c r="J32" s="200">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>24164.32</v>
+        <v>24796.81</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -36503,7 +36503,7 @@
       </c>
       <c r="J33" s="200">
         <f ca="1">'July 2027 - September 2027'!E136</f>
-        <v>24920.32</v>
+        <v>25552.81</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -36523,7 +36523,7 @@
       </c>
       <c r="J34" s="200">
         <f ca="1">'July 2027 - September 2027'!E163</f>
-        <v>25787.32</v>
+        <v>26419.81</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -36548,7 +36548,7 @@
       </c>
       <c r="J35" s="200">
         <f ca="1">'July 2027 - September 2027'!E190</f>
-        <v>26393.32</v>
+        <v>27025.81</v>
       </c>
     </row>
     <row r="36" ht="22" customHeight="1" spans="1:10">
@@ -36571,7 +36571,7 @@
       </c>
       <c r="J36" s="200">
         <f ca="1">'October 2027 - December 2027'!E136</f>
-        <v>27420.32</v>
+        <v>28052.81</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -36590,7 +36590,7 @@
       </c>
       <c r="J37" s="200">
         <f ca="1">'October 2027 - December 2027'!E163</f>
-        <v>28016.32</v>
+        <v>28648.81</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -36609,7 +36609,7 @@
       </c>
       <c r="J38" s="200">
         <f ca="1">'October 2027 - December 2027'!E190</f>
-        <v>29043.32</v>
+        <v>29675.81</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -36628,7 +36628,7 @@
       </c>
       <c r="J39" s="200">
         <f ca="1">'January 2028 - March 2028'!E136</f>
-        <v>29849.32</v>
+        <v>30481.81</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -36647,7 +36647,7 @@
       </c>
       <c r="J40" s="200">
         <f ca="1">'January 2028 - March 2028'!E163</f>
-        <v>30716.32</v>
+        <v>31348.81</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -36666,7 +36666,7 @@
       </c>
       <c r="J41" s="200">
         <f ca="1">'January 2028 - March 2028'!E190</f>
-        <v>31362.32</v>
+        <v>31994.81</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -36688,7 +36688,7 @@
       </c>
       <c r="J42" s="200">
         <f ca="1">'April 2028 - June 2028'!E136</f>
-        <v>32389.32</v>
+        <v>33021.81</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -36698,7 +36698,7 @@
       </c>
       <c r="J43" s="200">
         <f ca="1">'April 2028 - June 2028'!E163</f>
-        <v>34068.32</v>
+        <v>34700.81</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -36708,7 +36708,7 @@
       </c>
       <c r="J44" s="200">
         <f ca="1">'April 2028 - June 2028'!E190</f>
-        <v>35095.32</v>
+        <v>35727.81</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -36718,7 +36718,7 @@
       </c>
       <c r="J45" s="200">
         <f ca="1">'July 2028 - September 2028'!E136</f>
-        <v>35901.32</v>
+        <v>36533.81</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -36738,7 +36738,7 @@
       </c>
       <c r="J46" s="200">
         <f ca="1">'July 2028 - September 2028'!E163</f>
-        <v>36768.32</v>
+        <v>37400.81</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -36763,7 +36763,7 @@
       </c>
       <c r="J47" s="200">
         <f ca="1">'July 2028 - September 2028'!E190</f>
-        <v>37524.32</v>
+        <v>38156.81</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -36786,7 +36786,7 @@
       </c>
       <c r="J48" s="200">
         <f ca="1">'October 2028 - December 2028'!E136</f>
-        <v>38551.32</v>
+        <v>39183.81</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -36805,7 +36805,7 @@
       </c>
       <c r="J49" s="200">
         <f ca="1">'October 2028 - December 2028'!E163</f>
-        <v>39147.32</v>
+        <v>39779.81</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -36824,7 +36824,7 @@
       </c>
       <c r="J50" s="196">
         <f ca="1">'October 2028 - December 2028'!E190</f>
-        <v>40174.32</v>
+        <v>40806.81</v>
       </c>
     </row>
     <row r="51" ht="41.1" customHeight="1" spans="1:7">
@@ -38688,8 +38688,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="F179" sqref="F179"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -38726,7 +38726,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -38740,7 +38740,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1231.32</v>
+        <v>1863.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -38754,7 +38754,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1537.64</v>
+        <v>3850.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -38770,7 +38770,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -40428,7 +40428,7 @@
       </c>
       <c r="C104" s="106" cm="1">
         <f ca="1" t="array" ref="C104">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E137")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E164")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E191")))+SUM(E124+E151+E178))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C118")</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -40504,7 +40504,7 @@
       </c>
       <c r="C108" s="106">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -40520,7 +40520,7 @@
       </c>
       <c r="C109" s="106">
         <f ca="1">C108-C96</f>
-        <v>-334150.01</v>
+        <v>-333622.5</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -41461,7 +41461,7 @@
       </c>
       <c r="D178" s="149"/>
       <c r="E178" s="37">
-        <v>0</v>
+        <v>527.51</v>
       </c>
       <c r="F178" s="14"/>
       <c r="G178" s="14"/>
@@ -41528,7 +41528,7 @@
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
-        <v>760</v>
+        <v>0</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -41543,7 +41543,7 @@
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -41627,7 +41627,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1231.32</v>
+        <v>1863.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -42151,7 +42151,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -42165,7 +42165,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4171.32</v>
+        <v>4803.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -42179,7 +42179,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4477.64</v>
+        <v>6790.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -42195,7 +42195,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -43814,7 +43814,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -43890,7 +43890,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -43906,7 +43906,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -44000,7 +44000,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="89" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!E190")</f>
-        <v>1231.32</v>
+        <v>1863.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -44274,7 +44274,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>2258.32</v>
+        <v>2890.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -44366,7 +44366,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>2258.32</v>
+        <v>2890.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -44640,7 +44640,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3144.32</v>
+        <v>3776.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -44732,7 +44732,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>3144.32</v>
+        <v>3776.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -45006,7 +45006,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4171.32</v>
+        <v>4803.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -45571,7 +45571,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -45587,7 +45587,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>6890.32</v>
+        <v>7522.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -45603,7 +45603,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>7196.64</v>
+        <v>9509.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -45619,7 +45619,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -47238,7 +47238,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -47314,7 +47314,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -47330,7 +47330,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -47424,7 +47424,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!E190")</f>
-        <v>4171.32</v>
+        <v>4803.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -47698,7 +47698,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5107.32</v>
+        <v>5739.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -47790,7 +47790,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>5107.32</v>
+        <v>5739.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -48066,7 +48066,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>6084.32</v>
+        <v>6716.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -48158,7 +48158,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>6084.32</v>
+        <v>6716.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -48434,7 +48434,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6890.32</v>
+        <v>7522.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -49009,7 +49009,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -49025,7 +49025,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>9540.32</v>
+        <v>10172.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -49041,7 +49041,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>9846.64</v>
+        <v>12159.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -49057,7 +49057,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -50676,7 +50676,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -50752,7 +50752,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -50768,7 +50768,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -50862,7 +50862,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>6890.32</v>
+        <v>7522.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -51138,7 +51138,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>7917.32</v>
+        <v>8549.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -51230,7 +51230,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>7917.32</v>
+        <v>8549.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -51502,7 +51502,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>8513.32</v>
+        <v>9145.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -51594,7 +51594,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>8513.32</v>
+        <v>9145.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -51866,7 +51866,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>9540.32</v>
+        <v>10172.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -52399,7 +52399,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -52415,7 +52415,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>12902.32</v>
+        <v>13534.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -52431,7 +52431,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>13208.64</v>
+        <v>15521.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -52447,7 +52447,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -54070,7 +54070,7 @@
       </c>
       <c r="C104" s="106" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -54146,7 +54146,7 @@
       </c>
       <c r="C108" s="106">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -54162,7 +54162,7 @@
       </c>
       <c r="C109" s="106">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -54256,7 +54256,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>9540.32</v>
+        <v>10172.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -54528,7 +54528,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>10296.32</v>
+        <v>10928.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -54620,7 +54620,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>10296.32</v>
+        <v>10928.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -54892,7 +54892,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>12246.32</v>
+        <v>12878.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -54984,7 +54984,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>12246.32</v>
+        <v>12878.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -55256,7 +55256,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>12902.32</v>
+        <v>13534.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -55786,7 +55786,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>306.32</v>
+        <v>1986.81</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -55802,7 +55802,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>15552.32</v>
+        <v>16184.81</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -55818,7 +55818,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>15858.64</v>
+        <v>18171.62</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55834,7 +55834,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -57455,7 +57455,7 @@
       </c>
       <c r="C104" s="106" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-527.51</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -57531,7 +57531,7 @@
       </c>
       <c r="C108" s="106">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-333730.02</v>
+        <v>-333202.51</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -57547,7 +57547,7 @@
       </c>
       <c r="C109" s="106">
         <f ca="1">C108-C96</f>
-        <v>-334069.02</v>
+        <v>-333541.51</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -57641,7 +57641,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>12902.32</v>
+        <v>13534.81</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -57913,7 +57913,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>13929.32</v>
+        <v>14561.81</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -58005,7 +58005,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>13929.32</v>
+        <v>14561.81</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -58277,7 +58277,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14525.32</v>
+        <v>15157.81</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -58369,7 +58369,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>14525.32</v>
+        <v>15157.81</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -58641,7 +58641,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>15552.32</v>
+        <v>16184.81</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>